<commit_message>
latest feature extraction and cleaned up whole project
</commit_message>
<xml_diff>
--- a/utils/ParticipantOverviewAnonymized.xlsx
+++ b/utils/ParticipantOverviewAnonymized.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tzp466/Documents/code/copco-processing/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E16B09A-A641-6C41-998D-533220812EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE1735E-D77C-D241-8191-A65C71404E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="351">
   <si>
     <t>#</t>
   </si>
@@ -1060,9 +1060,6 @@
     <t>Course in B-C some years ago (doesn't remember well), but attended high school in Denmark for a year</t>
   </si>
   <si>
-    <t>possibly</t>
-  </si>
-  <si>
     <t>P55</t>
   </si>
   <si>
@@ -1145,6 +1142,27 @@
   </si>
   <si>
     <t>pseudohomophone_score</t>
+  </si>
+  <si>
+    <t>P58</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>26670, 12063, 22811, 26682</t>
+  </si>
+  <si>
+    <t>norrmal vision</t>
+  </si>
+  <si>
+    <t>4 years; Aug 2018 on sprogskole (had learned a bit prior)</t>
+  </si>
+  <si>
+    <t>Every day; speaking: 4, writing: 2, reading: 4, listening: 4</t>
+  </si>
+  <si>
+    <t>dansk3,6 (sprogskole); B2 (juni 2021)</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1346,6 +1364,9 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1564,10 +1585,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE67"/>
+  <dimension ref="A1:AF67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="M30" workbookViewId="0">
+      <selection activeCell="X45" sqref="X45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1601,19 +1622,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>5</v>
@@ -1628,7 +1649,7 @@
         <v>8</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>9</v>
@@ -1640,7 +1661,7 @@
         <v>11</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>12</v>
@@ -1655,10 +1676,10 @@
         <v>15</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Y1" s="5" t="s">
         <v>16</v>
@@ -1886,7 +1907,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>40</v>
@@ -4429,6 +4450,9 @@
       <c r="W40" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="X40">
+        <v>0.36842105263157893</v>
+      </c>
       <c r="Y40" s="6" t="s">
         <v>237</v>
       </c>
@@ -4503,6 +4527,9 @@
       <c r="W41" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="X41">
+        <v>0.15789473684210525</v>
+      </c>
       <c r="Y41" s="6" t="s">
         <v>243</v>
       </c>
@@ -4580,7 +4607,9 @@
       <c r="W42" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X42" s="6"/>
+      <c r="X42" s="6">
+        <v>0.26315789473684209</v>
+      </c>
       <c r="Y42" s="6" t="s">
         <v>251</v>
       </c>
@@ -4750,7 +4779,7 @@
         <v>23</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J45" s="6" t="s">
         <v>217</v>
@@ -4978,7 +5007,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="6">
         <v>49</v>
       </c>
@@ -5046,7 +5075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="6">
         <v>50</v>
       </c>
@@ -5114,7 +5143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="6">
         <v>51</v>
       </c>
@@ -5182,7 +5211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="6">
         <v>52</v>
       </c>
@@ -5250,7 +5279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="6">
         <v>53</v>
       </c>
@@ -5276,7 +5305,7 @@
         <v>48</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>34</v>
@@ -5318,7 +5347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="6">
         <v>54</v>
       </c>
@@ -5377,7 +5406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="6">
         <v>55</v>
       </c>
@@ -5442,10 +5471,10 @@
         <v>315</v>
       </c>
       <c r="W55" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="6">
         <v>56</v>
       </c>
@@ -5459,7 +5488,7 @@
         <v>81</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F56" s="6">
         <v>2</v>
@@ -5471,7 +5500,7 @@
         <v>48</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J56" s="6" t="s">
         <v>217</v>
@@ -5483,7 +5512,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="M56" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N56" s="6" t="s">
         <v>25</v>
@@ -5501,19 +5530,19 @@
         <v>57</v>
       </c>
       <c r="T56" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="U56" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="U56" s="6" t="s">
+      <c r="V56" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="V56" s="6" t="s">
-        <v>322</v>
-      </c>
       <c r="W56" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="6">
         <v>57</v>
       </c>
@@ -5527,7 +5556,7 @@
         <v>81</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F57" s="6">
         <v>2</v>
@@ -5539,7 +5568,7 @@
         <v>23</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>34</v>
@@ -5551,7 +5580,7 @@
         <v>0.71527777777777779</v>
       </c>
       <c r="M57" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N57" s="6" t="s">
         <v>25</v>
@@ -5569,19 +5598,19 @@
         <v>57</v>
       </c>
       <c r="T57" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="U57" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="U57" s="6" t="s">
+      <c r="V57" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="V57" s="6" t="s">
-        <v>328</v>
-      </c>
       <c r="W57" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="6">
         <v>58</v>
       </c>
@@ -5595,7 +5624,7 @@
         <v>81</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F58" s="6">
         <v>1</v>
@@ -5607,7 +5636,7 @@
         <v>23</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J58" s="6" t="s">
         <v>217</v>
@@ -5619,7 +5648,7 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="M58" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N58" s="6" t="s">
         <v>25</v>
@@ -5627,6 +5656,9 @@
       <c r="O58" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="Q58" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="R58" s="39">
         <v>1.7</v>
       </c>
@@ -5634,40 +5666,114 @@
         <v>57</v>
       </c>
       <c r="T58" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="U58" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="U58" s="6" t="s">
+      <c r="V58" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="V58" s="6" t="s">
-        <v>334</v>
-      </c>
       <c r="W58" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="13" x14ac:dyDescent="0.15">
-      <c r="B59" s="34"/>
-      <c r="C59" s="29"/>
-    </row>
-    <row r="60" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:32" ht="13" x14ac:dyDescent="0.15">
+      <c r="A59" s="41">
+        <v>59</v>
+      </c>
+      <c r="B59" s="42">
+        <v>44823</v>
+      </c>
+      <c r="C59" s="43">
+        <v>0.625</v>
+      </c>
+      <c r="D59" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E59" s="41" t="s">
+        <v>344</v>
+      </c>
+      <c r="F59" s="41">
+        <v>1</v>
+      </c>
+      <c r="G59" s="41">
+        <v>32</v>
+      </c>
+      <c r="H59" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="I59" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="J59" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K59" s="43">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="L59" s="43">
+        <v>0.6875</v>
+      </c>
+      <c r="M59" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="N59" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="O59" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="P59" s="41"/>
+      <c r="Q59" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="R59" s="39">
+        <v>1.2</v>
+      </c>
+      <c r="S59" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="T59" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="U59" s="41" t="s">
+        <v>349</v>
+      </c>
+      <c r="V59" s="41" t="s">
+        <v>350</v>
+      </c>
+      <c r="W59" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="X59" s="41"/>
+      <c r="Y59" s="41"/>
+      <c r="Z59" s="41"/>
+      <c r="AA59" s="41"/>
+      <c r="AB59" s="41"/>
+      <c r="AC59" s="41"/>
+      <c r="AD59" s="41"/>
+      <c r="AE59" s="41"/>
+      <c r="AF59" s="41"/>
+    </row>
+    <row r="60" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="E60" s="15"/>
       <c r="F60" s="38"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
       <c r="I60" s="15"/>
     </row>
-    <row r="62" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="B62" s="6"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="B63" s="6"/>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:23" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="B64" s="34"/>
       <c r="C64" s="29"/>
       <c r="H64" s="6"/>

</xml_diff>